<commit_message>
updated slides and additional appendix for regression tables
</commit_message>
<xml_diff>
--- a/Tables/PCA_ab_reason_bought.xlsx
+++ b/Tables/PCA_ab_reason_bought.xlsx
@@ -90,13 +90,13 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>0.42171312516158349</v>
+        <v>0.42171312516158316</v>
       </c>
       <c r="C1">
-        <v>-0.43379680561591605</v>
+        <v>-0.43379680561591683</v>
       </c>
       <c r="D1">
-        <v>-0.031257780519316263</v>
+        <v>-0.031257780519314236</v>
       </c>
     </row>
     <row r="2">
@@ -104,13 +104,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.4426528668435728</v>
+        <v>0.44265286684357258</v>
       </c>
       <c r="C2">
-        <v>0.019269734114618107</v>
+        <v>0.019269734114618776</v>
       </c>
       <c r="D2">
-        <v>-0.1081395859809894</v>
+        <v>-0.10813958598099302</v>
       </c>
     </row>
     <row r="3">
@@ -118,13 +118,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.40322573496594749</v>
+        <v>0.40322573496594799</v>
       </c>
       <c r="C3">
-        <v>0.19165489434818039</v>
+        <v>0.19165489434818112</v>
       </c>
       <c r="D3">
-        <v>-0.22869103566190122</v>
+        <v>-0.22869103566190024</v>
       </c>
     </row>
     <row r="4">
@@ -132,13 +132,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.29623339399397686</v>
+        <v>0.29623339399397741</v>
       </c>
       <c r="C4">
-        <v>0.28212925862930277</v>
+        <v>0.28212925862930255</v>
       </c>
       <c r="D4">
-        <v>0.62263542865576804</v>
+        <v>0.62263542865576949</v>
       </c>
     </row>
     <row r="5">
@@ -146,13 +146,13 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.33634285027750327</v>
+        <v>0.33634285027750349</v>
       </c>
       <c r="C5">
-        <v>0.30722099791121865</v>
+        <v>0.3072209979112181</v>
       </c>
       <c r="D5">
-        <v>-0.23343798287691606</v>
+        <v>-0.23343798287691586</v>
       </c>
     </row>
     <row r="6">
@@ -160,13 +160,13 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.3083680692434525</v>
+        <v>0.30836806924345272</v>
       </c>
       <c r="C6">
-        <v>0.44399742168628181</v>
+        <v>0.4439974216862802</v>
       </c>
       <c r="D6">
-        <v>-0.22598156553865897</v>
+        <v>-0.22598156553865947</v>
       </c>
     </row>
     <row r="7">
@@ -174,13 +174,13 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.30934131516956315</v>
+        <v>0.30934131516956198</v>
       </c>
       <c r="C7">
-        <v>-0.21415210211212787</v>
+        <v>-0.21415210211212682</v>
       </c>
       <c r="D7">
-        <v>0.60907130715445867</v>
+        <v>0.60907130715445879</v>
       </c>
     </row>
     <row r="8">
@@ -188,13 +188,13 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>-0.26825703001605178</v>
+        <v>-0.26825703001605145</v>
       </c>
       <c r="C8">
-        <v>0.59811446799218482</v>
+        <v>0.59811446799218582</v>
       </c>
       <c r="D8">
-        <v>0.26613060192246429</v>
+        <v>0.26613060192246335</v>
       </c>
     </row>
   </sheetData>
@@ -211,10 +211,10 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>0.056296338653494933</v>
+        <v>0.056296338653494524</v>
       </c>
       <c r="C1">
-        <v>0.58451696640924389</v>
+        <v>0.58451696640924344</v>
       </c>
       <c r="D1">
         <v>0.14889363845732997</v>
@@ -225,13 +225,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.36635714533481623</v>
+        <v>0.36635714533481845</v>
       </c>
       <c r="C2">
-        <v>0.24646697905583528</v>
+        <v>0.24646697905583465</v>
       </c>
       <c r="D2">
-        <v>0.11420824633552751</v>
+        <v>0.11420824633552375</v>
       </c>
     </row>
     <row r="3">
@@ -239,13 +239,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.48841929326789291</v>
+        <v>0.48841929326789363</v>
       </c>
       <c r="C3">
-        <v>0.11430588903632805</v>
+        <v>0.11430588903632621</v>
       </c>
       <c r="D3">
-        <v>-0.0017144543914459354</v>
+        <v>-0.0017144543914448807</v>
       </c>
     </row>
     <row r="4">
@@ -253,13 +253,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.11749007937062794</v>
+        <v>0.11749007937062678</v>
       </c>
       <c r="C4">
-        <v>-0.21915897322031938</v>
+        <v>-0.21915897322031724</v>
       </c>
       <c r="D4">
-        <v>0.70227590376985172</v>
+        <v>0.70227590376985394</v>
       </c>
     </row>
     <row r="5">
@@ -267,13 +267,13 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.51070207015855684</v>
+        <v>0.51070207015855673</v>
       </c>
       <c r="C5">
-        <v>-0.014024191544848172</v>
+        <v>-0.014024191544848928</v>
       </c>
       <c r="D5">
-        <v>-0.031484344161521932</v>
+        <v>-0.031484344161521349</v>
       </c>
     </row>
     <row r="6">
@@ -281,13 +281,13 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.56766766950766501</v>
+        <v>0.56766766950766423</v>
       </c>
       <c r="C6">
-        <v>-0.14169857803588115</v>
+        <v>-0.14169857803588087</v>
       </c>
       <c r="D6">
-        <v>-0.031099429812288859</v>
+        <v>-0.031099429812288554</v>
       </c>
     </row>
     <row r="7">
@@ -295,13 +295,13 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-0.15680609886235952</v>
+        <v>-0.15680609886235986</v>
       </c>
       <c r="C7">
-        <v>0.19368802067615215</v>
+        <v>0.19368802067615276</v>
       </c>
       <c r="D7">
-        <v>0.67113175108531564</v>
+        <v>0.67113175108531453</v>
       </c>
     </row>
     <row r="8">
@@ -309,13 +309,13 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.051034296513023783</v>
+        <v>0.051034296513023561</v>
       </c>
       <c r="C8">
-        <v>-0.69188672344837976</v>
+        <v>-0.69188672344837909</v>
       </c>
       <c r="D8">
-        <v>0.13862362983815807</v>
+        <v>0.13862362983815943</v>
       </c>
     </row>
   </sheetData>
@@ -332,13 +332,13 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>0.044669686160138805</v>
+        <v>0.044669686160139027</v>
       </c>
       <c r="C1">
-        <v>-0.57847146711824005</v>
+        <v>-0.5784714671182396</v>
       </c>
       <c r="D1">
-        <v>0.12651599284593279</v>
+        <v>0.12651599284593296</v>
       </c>
     </row>
     <row r="2">
@@ -346,13 +346,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.36044373046733885</v>
+        <v>0.36044373046734152</v>
       </c>
       <c r="C2">
-        <v>-0.23811672530351391</v>
+        <v>-0.23811672530351358</v>
       </c>
       <c r="D2">
-        <v>0.10044090380256956</v>
+        <v>0.10044090380256618</v>
       </c>
     </row>
     <row r="3">
@@ -360,13 +360,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.48716833466923554</v>
+        <v>0.48716833466923642</v>
       </c>
       <c r="C3">
-        <v>-0.10994820883749098</v>
+        <v>-0.10994820883748928</v>
       </c>
       <c r="D3">
-        <v>-0.012494094664978098</v>
+        <v>-0.012494094664976491</v>
       </c>
     </row>
     <row r="4">
@@ -374,13 +374,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.10394948335993945</v>
+        <v>0.10394948335993903</v>
       </c>
       <c r="C4">
-        <v>0.25454608383985694</v>
+        <v>0.25454608383985483</v>
       </c>
       <c r="D4">
-        <v>0.71156018884807848</v>
+        <v>0.7115601888480807</v>
       </c>
     </row>
     <row r="5">
@@ -391,10 +391,10 @@
         <v>0.51195560719970823</v>
       </c>
       <c r="C5">
-        <v>0.017531954389663425</v>
+        <v>0.017531954389664022</v>
       </c>
       <c r="D5">
-        <v>-0.037797152392436278</v>
+        <v>-0.037797152392435168</v>
       </c>
     </row>
     <row r="6">
@@ -402,13 +402,13 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.57072238242968854</v>
+        <v>0.57072238242968765</v>
       </c>
       <c r="C6">
-        <v>0.14613656671525352</v>
+        <v>0.14613656671525305</v>
       </c>
       <c r="D6">
-        <v>-0.033319212332070892</v>
+        <v>-0.033319212332070067</v>
       </c>
     </row>
     <row r="7">
@@ -416,13 +416,13 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-0.17551662792501219</v>
+        <v>-0.17551662792501149</v>
       </c>
       <c r="C7">
-        <v>-0.16361854322461172</v>
+        <v>-0.16361854322461233</v>
       </c>
       <c r="D7">
-        <v>0.66826108441526788</v>
+        <v>0.66826108441526655</v>
       </c>
     </row>
     <row r="8">
@@ -430,13 +430,13 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.057398838598889099</v>
+        <v>0.05739883859888855</v>
       </c>
       <c r="C8">
-        <v>0.70095541244345383</v>
+        <v>0.70095541244345316</v>
       </c>
       <c r="D8">
-        <v>0.16469084235182496</v>
+        <v>0.16469084235182621</v>
       </c>
     </row>
   </sheetData>

</xml_diff>